<commit_message>
comfirm: 71.2% for ide, 75.2% for PCB
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnny\Documents\Github\open-reid-PCB_n_RPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hou_yz\Documents\GitHub\open-reid-PCB_n_RPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,33 +25,71 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
   <si>
-    <t>softmax optimizer + 256 dim feat</t>
-  </si>
-  <si>
     <t>NO randcrop + 0.5 drop after feat + feat init</t>
   </si>
   <si>
-    <t>origianl optimizer + 1536 dim feat</t>
-  </si>
-  <si>
-    <t>softmax optimizer + 1536 dim feat</t>
+    <t>softmax optimizer (stepsize=50) + 256 dim feat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>origianl optimizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>softmax optimizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NO randcrop + 0.5 drop after feat + feat init + 1536dim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>momentum + original -lr adjust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>momentum + nestrov + original -lr adjust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>softmax optimizer (stepsize=40) + 256 dim feat, repeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>softmax optimizer (stepsize=40) + 256 dim feat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corrupt?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corrupt?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -75,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -85,9 +123,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -103,7 +142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -365,25 +404,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="44.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -391,18 +431,52 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>0.72499999999999998</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.71199999999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -410,25 +484,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -436,18 +510,35 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>0.72199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.746</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dropout move to after pool5
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21888" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21888" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ide" sheetId="1" r:id="rId1"/>
     <sheet name="pcb" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>softmax optimizer + 751 dim feat</t>
   </si>
@@ -70,6 +71,30 @@
   </si>
   <si>
     <t>corrupt?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>softmax optimizer (stepsize=40) + 256 dim feat + droup after pool5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>corrupt?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>momentum + nestrov + original -lr adjust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drop after pool5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>momentum + nestrov + original -lr adjust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>softmax optimizer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -120,10 +145,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -404,24 +429,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -470,6 +496,14 @@
       </c>
       <c r="B6" s="3">
         <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.71899999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -484,25 +518,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -510,7 +544,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -518,27 +552,65 @@
         <v>0.72199999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>0.752</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.746</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.745</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.74</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.63200000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>